<commit_message>
Added new ideas for how to pass through a CAN / USB Device to Docker (especially with UDEV)
</commit_message>
<xml_diff>
--- a/strategy/2024-02-25.xlsx
+++ b/strategy/2024-02-25.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,7 +846,7 @@
         <v>45347.6666550926</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">$H$3</f>

</xml_diff>

<commit_message>
Explained more in detail how CAN Interface Names and USB Devices Names can be changed to something that can survive reboots, device disconnection-reconnection, etc
</commit_message>
<xml_diff>
--- a/strategy/2024-02-25.xlsx
+++ b/strategy/2024-02-25.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -819,7 +819,7 @@
         <v>45347.6249884259</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H17" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -846,7 +846,7 @@
         <v>45347.6666550926</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>55</v>
+        <v>55.5</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">$H$3</f>

</xml_diff>